<commit_message>
Doc, Test Sheet and comments fix up.
</commit_message>
<xml_diff>
--- a/workings/eithne_test_sheet.xlsx
+++ b/workings/eithne_test_sheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://galwaymayoinstitute-my.sharepoint.com/personal/g00348436_gmit_ie/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnd\OneDrive\Desktop\Home\_Projects\Eithne-Voice-Assistant\workings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24791E59-10EB-4D76-876B-42029F7EB58B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{11688FB3-9311-4F5F-90B2-EF86B7E4E067}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5790" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="App Test Sheet" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,17 +36,11 @@
     <t>Purpose:</t>
   </si>
   <si>
-    <t xml:space="preserve">This set of tests is intended to check that the Application has its main functionalites.                </t>
-  </si>
-  <si>
     <t>Gesture Based UI Development                                               John Shields - G00348436 
 'Eithne Voice Assistant'            
 Test Sheet of the Application.</t>
   </si>
   <si>
-    <t>This Application was tested thourgh the Command-Line and the Google Chrome Browser.</t>
-  </si>
-  <si>
     <t>Requirement  ID</t>
   </si>
   <si>
@@ -86,9 +80,6 @@
   </si>
   <si>
     <t>Run App</t>
-  </si>
-  <si>
-    <t>App Functionailty</t>
   </si>
   <si>
     <t>•In the App's directory  in CLI enter:              python main.py</t>
@@ -256,9 +247,6 @@
     <t>History of Today</t>
   </si>
   <si>
-    <t>Histroy of Today Feature</t>
-  </si>
-  <si>
     <t xml:space="preserve">• Say one of the following into Microphone:                                                                                      • History                                                                                                                      • What happened today                                                                                                                                                                  •  History of Today                                                                                        </t>
   </si>
   <si>
@@ -280,9 +268,6 @@
   </si>
   <si>
     <t>YouTube Query Feature</t>
-  </si>
-  <si>
-    <t>• Say one of the following into Microphone:         Part 1:                                                                                             • YuTube, Video or Open YouTube                                                                                                                               • I would like to watch a video                                                                       Part 2:                                                                                             •  Say an input for a YouTube Query e.g: Jazz Music</t>
   </si>
   <si>
     <t>User input is recognized and Eithne responds by asking what the user would like to search for. Then User says "Jazz Music" and Eithne does a YouTube Query for Jazz Music</t>
@@ -312,67 +297,82 @@
     <t>• Say one of the following into Microphone:         Part 1:                                                                                             •  Website, surf the web internet or online                                                                                                                              •                                                                                                       Part 2:                                                                                             •  Say an input for a website e.g: GitHub</t>
   </si>
   <si>
-    <t>User input is recognized and Eithne responds by asking what website would they like to vist. Then User says "GitHub" and Eithne loads the browser with said website</t>
+    <t>TC.012</t>
+  </si>
+  <si>
+    <t>Invalid/no input</t>
+  </si>
+  <si>
+    <t>Invalid/no input handing</t>
+  </si>
+  <si>
+    <t>• Say a gibberish word into Microphone</t>
+  </si>
+  <si>
+    <t>User input is not recognized and Eithne notifies them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• User input is not recognized and Eithne notifies them                                                                                                                        </t>
+  </si>
+  <si>
+    <t>User input was not recognized and Eithne notified them</t>
+  </si>
+  <si>
+    <t>Turn off Eithne</t>
+  </si>
+  <si>
+    <t>Turn off Functionality</t>
+  </si>
+  <si>
+    <t>• Say one of the following into Microphone:                                                                                      •  Turn off                                                                                                                     • Stop listening                                                                                                                                                                 •  Exit                                                                                               • Quit</t>
+  </si>
+  <si>
+    <t>User input is recognized, Eithne says her goodbyes and turns off</t>
   </si>
   <si>
     <t xml:space="preserve">• User input is recognized                                                               
-• Eithne responds by asking what website would the user like to vist                                                            
+• Eithne says her goodbyes and turns off                                                                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• User input was recognized                                                               
+• Eithne said her goodbyes and turned off                                                                                         </t>
+  </si>
+  <si>
+    <t>This Application was tested through the Command-Line and the Google Chrome Browser.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This set of tests is intended to check that the Application has all its main functionalities in working order.                </t>
+  </si>
+  <si>
+    <t>History of Today Feature</t>
+  </si>
+  <si>
+    <t>• Say one of the following into Microphone:         Part 1:                                                                                             • YouTube, Video or Open YouTube                                                                                                                               • I would like to watch a video                                                                       Part 2:                                                                                             •  Say an input for a YouTube Query e.g: Jazz Music</t>
+  </si>
+  <si>
+    <t>User input is recognized and Eithne responds by asking what website would they like to visit. Then User says "GitHub" and Eithne loads the browser with said website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• User input is recognized                                                               
+• Eithne responds by asking what website would the user like to visit                                                            
 •  Then User says "GitHub"                          
 • Eithne loads the browser with said website                                                                                                      </t>
   </si>
   <si>
     <t xml:space="preserve">• User input was recognized                                                               
-• Eithne responded by asking what website would the user like to vist                                                            
+• Eithne responded by asking what website would the user like to visit                                                            
 •  Then User said "GitHub"                          
 • Eithne loaded the browser with said website          </t>
   </si>
   <si>
-    <t>TC.012</t>
-  </si>
-  <si>
-    <t>Invalid/no input</t>
-  </si>
-  <si>
-    <t>Invalid/no input handing</t>
-  </si>
-  <si>
-    <t>• Say a gibberish word into Microphone</t>
-  </si>
-  <si>
-    <t>User input is not recognized and Eithne notifies them</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• User input is not recognized and Eithne notifies them                                                                                                                        </t>
-  </si>
-  <si>
-    <t>User input was not recognized and Eithne notified them</t>
-  </si>
-  <si>
-    <t>Turn off Eithne</t>
-  </si>
-  <si>
-    <t>Turn off Functionality</t>
-  </si>
-  <si>
-    <t>• Say one of the following into Microphone:                                                                                      •  Turn off                                                                                                                     • Stop listening                                                                                                                                                                 •  Exit                                                                                               • Quit</t>
-  </si>
-  <si>
-    <t>User input is recognized, Eithne says her goodbyes and turns off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• User input is recognized                                                               
-• Eithne says her goodbyes and turns off                                                                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">• User input was recognized                                                               
-• Eithne said her goodbyes and turned off                                                                                         </t>
+    <t>App Functionality</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,11 +1008,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="3" width="20.7109375" customWidth="1"/>
@@ -1026,25 +1026,25 @@
     <col min="12" max="12" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="56.25" customHeight="1">
+    <row r="1" spans="1:12" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="C1" s="17"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="150" customHeight="1" thickBot="1">
+    <row r="2" spans="1:12" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
       <c r="D2" s="20"/>
       <c r="E2" s="14" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="1"/>
@@ -1053,42 +1053,42 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="49.5" customHeight="1">
+    <row r="3" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="69.95" customHeight="1">
+    </row>
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1096,32 +1096,32 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:12" s="7" customFormat="1" ht="95.1" customHeight="1">
+    <row r="5" spans="1:12" s="7" customFormat="1" ht="95.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -1129,32 +1129,32 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="H5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="I5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>29</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:12" s="7" customFormat="1" ht="99.95" customHeight="1">
+    <row r="6" spans="1:12" s="7" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1162,32 +1162,32 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="H6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="J6" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:12" s="7" customFormat="1" ht="80.099999999999994" customHeight="1">
+    <row r="7" spans="1:12" s="7" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -1195,32 +1195,32 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="H7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="J7" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:12" s="7" customFormat="1" ht="120" customHeight="1">
+    <row r="8" spans="1:12" s="7" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -1228,32 +1228,32 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="H8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="I8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:12" s="7" customFormat="1" ht="110.1" customHeight="1">
+    <row r="9" spans="1:12" s="7" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -1261,32 +1261,32 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="I9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="J9" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:12" s="7" customFormat="1" ht="110.1" customHeight="1">
+    <row r="10" spans="1:12" s="7" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>8</v>
       </c>
@@ -1294,32 +1294,32 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="H10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="J10" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:12" s="7" customFormat="1" ht="84.95" customHeight="1">
+    <row r="11" spans="1:12" s="7" customFormat="1" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>9</v>
       </c>
@@ -1327,32 +1327,32 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="H11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="I11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="J11" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:12" s="7" customFormat="1" ht="110.1" customHeight="1">
+    <row r="12" spans="1:12" s="7" customFormat="1" ht="110.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>10</v>
       </c>
@@ -1360,32 +1360,32 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="I12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="J12" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:12" s="7" customFormat="1" ht="99.95" customHeight="1">
+    <row r="13" spans="1:12" s="7" customFormat="1" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>11</v>
       </c>
@@ -1393,32 +1393,32 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:12" s="7" customFormat="1" ht="54.95" customHeight="1">
+    <row r="14" spans="1:12" s="7" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>12</v>
       </c>
@@ -1426,32 +1426,32 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:12" s="7" customFormat="1" ht="114.95" customHeight="1">
+    <row r="15" spans="1:12" s="7" customFormat="1" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>13</v>
       </c>
@@ -1459,33 +1459,33 @@
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="1:12" s="7" customFormat="1" ht="129.94999999999999" customHeight="1">
+    <row r="16" spans="1:12" s="7" customFormat="1" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1499,7 +1499,7 @@
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:12" s="7" customFormat="1">
+    <row r="17" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1513,7 +1513,7 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="18" spans="1:12" s="7" customFormat="1">
+    <row r="18" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1527,7 +1527,7 @@
       <c r="K18"/>
       <c r="L18"/>
     </row>
-    <row r="19" spans="1:12" s="7" customFormat="1">
+    <row r="19" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1541,7 +1541,7 @@
       <c r="K19"/>
       <c r="L19"/>
     </row>
-    <row r="20" spans="1:12" s="7" customFormat="1">
+    <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1555,7 +1555,7 @@
       <c r="K20"/>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" s="7" customFormat="1">
+    <row r="21" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1569,7 +1569,7 @@
       <c r="K21"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:12" s="7" customFormat="1">
+    <row r="22" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1583,7 +1583,7 @@
       <c r="K22"/>
       <c r="L22"/>
     </row>
-    <row r="23" spans="1:12" s="7" customFormat="1">
+    <row r="23" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1597,7 +1597,7 @@
       <c r="K23"/>
       <c r="L23"/>
     </row>
-    <row r="24" spans="1:12" s="7" customFormat="1">
+    <row r="24" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1611,7 +1611,7 @@
       <c r="K24"/>
       <c r="L24"/>
     </row>
-    <row r="25" spans="1:12" s="7" customFormat="1">
+    <row r="25" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -1625,7 +1625,7 @@
       <c r="K25"/>
       <c r="L25"/>
     </row>
-    <row r="26" spans="1:12" s="7" customFormat="1">
+    <row r="26" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -1639,7 +1639,7 @@
       <c r="K26"/>
       <c r="L26"/>
     </row>
-    <row r="27" spans="1:12" s="7" customFormat="1">
+    <row r="27" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -1653,7 +1653,7 @@
       <c r="K27"/>
       <c r="L27"/>
     </row>
-    <row r="28" spans="1:12" s="7" customFormat="1">
+    <row r="28" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -1667,7 +1667,7 @@
       <c r="K28"/>
       <c r="L28"/>
     </row>
-    <row r="29" spans="1:12" s="7" customFormat="1">
+    <row r="29" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -1681,7 +1681,7 @@
       <c r="K29"/>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" s="7" customFormat="1">
+    <row r="30" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -1932,12 +1932,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1946,14 +1940,52 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BCFADAC-0F95-4DF3-9C08-7D2A00BAF868}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BCFADAC-0F95-4DF3-9C08-7D2A00BAF868}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="112c7e96-3675-4162-94bd-d5cbb4681c6c"/>
+    <ds:schemaRef ds:uri="aa346678-56a6-456f-9a38-432177ef9c3a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787BAD58-35B4-4E16-B7E4-7B790AB56F1E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AA35423-B04C-452A-B7E9-1D1C97DE04ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AA35423-B04C-452A-B7E9-1D1C97DE04ED}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{787BAD58-35B4-4E16-B7E4-7B790AB56F1E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="112c7e96-3675-4162-94bd-d5cbb4681c6c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa346678-56a6-456f-9a38-432177ef9c3a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>